<commit_message>
J'ai fait les évènements mais pas final besoin d'aide
</commit_message>
<xml_diff>
--- a/evenements.xlsx
+++ b/evenements.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Évènement</t>
   </si>
@@ -48,25 +48,77 @@
   </si>
   <si>
     <t>Client</t>
-  </si>
-  <si>
-    <t>Vérification de la
-commande</t>
   </si>
   <si>
     <t>Le client passe
 une commande</t>
   </si>
   <si>
-    <t>Une nouvelle commande
-est créée</t>
-  </si>
-  <si>
-    <t>Une erreur dans la
+    <t>Vérification de la
+nouvelle commande</t>
+  </si>
+  <si>
+    <t>Confirmation</t>
+  </si>
+  <si>
+    <t>La commande
+est refusée</t>
+  </si>
+  <si>
+    <t>Erreur dans la
 commande</t>
   </si>
   <si>
-    <t>Erreur dans commande</t>
+    <t>Pharmacien</t>
+  </si>
+  <si>
+    <t>Envoie une demande 
+de modification au
+client</t>
+  </si>
+  <si>
+    <t>Plus de 10min après
+la demande de 
+modification</t>
+  </si>
+  <si>
+    <t>Annule la commande</t>
+  </si>
+  <si>
+    <t>Cancellation de la
+commande</t>
+  </si>
+  <si>
+    <t>Refuse la modification</t>
+  </si>
+  <si>
+    <t>Modification dans
+la commande</t>
+  </si>
+  <si>
+    <t>Modifie la commande</t>
+  </si>
+  <si>
+    <t>Demande de 
+modification</t>
+  </si>
+  <si>
+    <t>Accepte la
+modification</t>
+  </si>
+  <si>
+    <t>Chargement de la
+commande</t>
+  </si>
+  <si>
+    <t>La commande est prête</t>
+  </si>
+  <si>
+    <t>Confirmation de
+reception</t>
+  </si>
+  <si>
+    <t>Alert de départ iminant</t>
   </si>
 </sst>
 </file>
@@ -116,12 +168,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -438,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8971EB09-101D-430D-A6E1-F005B92A0081}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,48 +506,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
+    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>